<commit_message>
Add more sentiment vs px ch graphs
</commit_message>
<xml_diff>
--- a/data/general/themes.xlsx
+++ b/data/general/themes.xlsx
@@ -209,9 +209,6 @@
     <t>MOVEMENT_SOCIAL</t>
   </si>
   <si>
-    <t>MOVEMENT_WOMENSd</t>
-  </si>
-  <si>
     <t>TRIAL</t>
   </si>
   <si>
@@ -231,6 +228,9 @@
   </si>
   <si>
     <t>LEAD</t>
+  </si>
+  <si>
+    <t>MOVEMENT_WOMENS</t>
   </si>
 </sst>
 </file>
@@ -548,7 +548,7 @@
   <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -560,22 +560,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" t="s">
         <v>62</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>63</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E1" t="s">
         <v>64</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>66</v>
-      </c>
-      <c r="E1" t="s">
-        <v>65</v>
-      </c>
-      <c r="F1" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -623,7 +623,7 @@
         <v>51</v>
       </c>
       <c r="E4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -678,7 +678,7 @@
         <v>34</v>
       </c>
       <c r="C9" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">

</xml_diff>